<commit_message>
Commit previous WIP for hospitalisations
</commit_message>
<xml_diff>
--- a/data/hospital-mortality-rates/percent_oldies_being_admitted_for_covid.xlsx
+++ b/data/hospital-mortality-rates/percent_oldies_being_admitted_for_covid.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Downloads\_covid_19\data\phe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WCA\covid-stats\data\hospital-mortality-rates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6CD03E-338D-4146-A927-CDD2F2C50A8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784F203B-9C5F-4F66-989D-1E0547882951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{4FDBA1C6-DBB4-4781-8CD2-40EB46E31092}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4FDBA1C6-DBB4-4781-8CD2-40EB46E31092}"/>
   </bookViews>
   <sheets>
     <sheet name="population" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
   <si>
     <t>0 to 4</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>ERD</t>
+  </si>
+  <si>
+    <t>POPULATION OF ENGLAND</t>
   </si>
 </sst>
 </file>
@@ -9234,11 +9237,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E4327BD-D7A4-4147-ADED-73CC8C3D888B}">
   <dimension ref="A1:IT20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11458,6 +11461,11 @@
       <c r="IS5" s="15"/>
       <c r="IT5" s="15"/>
     </row>
+    <row r="7" spans="1:254" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="8" spans="1:254" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>0</v>
@@ -11532,25 +11540,26 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B20" s="17">
         <f>B15-B5</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="B8:B14" formulaRange="1"/>
   </ignoredErrors>
@@ -12298,7 +12307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05DB733-493E-4AFB-AF78-ECABBDF05462}">
   <dimension ref="A1:AP29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="X21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>